<commit_message>
Lending Stuff App Update
</commit_message>
<xml_diff>
--- a/MSCW.xlsx
+++ b/MSCW.xlsx
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>